<commit_message>
Verificando se o arquivo é válido
</commit_message>
<xml_diff>
--- a/test_update.xlsx
+++ b/test_update.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="8">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">idade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
   </si>
   <si>
     <t xml:space="preserve">WHERE</t>
@@ -47,8 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -115,12 +119,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,13 +149,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -159,401 +167,512 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="C2" s="2" t="n">
+        <v>44053</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+      <c r="C3" s="2" t="n">
+        <v>44054</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
+      <c r="C4" s="2" t="n">
+        <v>44055</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
+      <c r="C5" s="2" t="n">
+        <v>44056</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
+      <c r="C6" s="2" t="n">
+        <v>44057</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
+      <c r="C7" s="2" t="n">
+        <v>44058</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
+      <c r="C8" s="2" t="n">
+        <v>44059</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
+      <c r="C9" s="2" t="n">
+        <v>44060</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
+      <c r="C10" s="2" t="n">
+        <v>44061</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
+      <c r="C11" s="2" t="n">
+        <v>44062</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="n">
+        <v>44063</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
+      <c r="C13" s="2" t="n">
+        <v>44064</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
+      <c r="C14" s="2" t="n">
+        <v>44065</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
+      <c r="C15" s="2" t="n">
+        <v>44066</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
+      <c r="C16" s="2" t="n">
+        <v>44067</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
+      <c r="C17" s="2" t="n">
+        <v>44068</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
+      <c r="C18" s="2" t="n">
+        <v>44069</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
+      <c r="C19" s="2" t="n">
+        <v>44070</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
+      <c r="C20" s="2" t="n">
+        <v>44071</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
+      <c r="C21" s="2" t="n">
+        <v>44072</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
+      <c r="C22" s="2" t="n">
+        <v>44073</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
+      <c r="C23" s="2" t="n">
+        <v>44074</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
+      <c r="C24" s="2" t="n">
+        <v>44075</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
+      <c r="C25" s="2" t="n">
+        <v>44076</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
+      <c r="C26" s="2" t="n">
+        <v>44077</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
+      <c r="C27" s="2" t="n">
+        <v>44078</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>4</v>
+      <c r="C28" s="2" t="n">
+        <v>44079</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
+      <c r="C29" s="2" t="n">
+        <v>44080</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>4</v>
+      <c r="C30" s="2" t="n">
+        <v>44081</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
+      <c r="C31" s="2" t="n">
+        <v>44082</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>4</v>
+      <c r="C32" s="2" t="n">
+        <v>44083</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
+      <c r="C33" s="2" t="n">
+        <v>44084</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>4</v>
+      <c r="C34" s="2" t="n">
+        <v>44085</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>6</v>
+      <c r="C35" s="2" t="n">
+        <v>44086</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
+      <c r="C36" s="2" t="n">
+        <v>44087</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>6</v>
+        <v>123.1231</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>44088</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>